<commit_message>
Project: LinkedIn Visuals Script: findEmployeeCount Test Status: updated Feature: common driver Feature Status: completed
</commit_message>
<xml_diff>
--- a/src/test/resources/linkedInVisuals/Linkedin Visuals_Omkar.xlsx
+++ b/src/test/resources/linkedInVisuals/Linkedin Visuals_Omkar.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Raymond James</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>15509</t>
-  </si>
-  <si>
     <t>57501</t>
   </si>
   <si>
@@ -81,13 +78,22 @@
     <t>139</t>
   </si>
   <si>
-    <t>10001</t>
-  </si>
-  <si>
     <t>1,001-5,000</t>
   </si>
   <si>
     <t>10001+</t>
+  </si>
+  <si>
+    <t>15515</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>57474</t>
+  </si>
+  <si>
+    <t>86317</t>
   </si>
 </sst>
 </file>
@@ -151,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -159,42 +165,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -542,10 +512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,13 +562,13 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -610,13 +580,13 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -628,13 +598,13 @@
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="6"/>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -646,17 +616,13 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[2] Project: LinkedIn Visuals Script: findEmployeeCount Test Status: updated Feature: common driver Feature Status: completed
</commit_message>
<xml_diff>
--- a/src/test/resources/linkedInVisuals/Linkedin Visuals_Omkar.xlsx
+++ b/src/test/resources/linkedInVisuals/Linkedin Visuals_Omkar.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>Raymond James</t>
   </si>
@@ -69,6 +69,9 @@
     <t>Chrome</t>
   </si>
   <si>
+    <t>15509</t>
+  </si>
+  <si>
     <t>57501</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
   </si>
   <si>
     <t>139</t>
+  </si>
+  <si>
+    <t>10001</t>
   </si>
   <si>
     <t>1,001-5,000</t>
@@ -157,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -165,6 +171,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -512,10 +602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,13 +652,13 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2"/>
+      <c r="D3" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -580,13 +670,13 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="D4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -598,13 +688,13 @@
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="D5" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -616,13 +706,17 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="D6" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[3] Project: LinkedIn Visuals Script: findEmployeeCount Test Status: updated Feature: common driver Feature Status: completed
</commit_message>
<xml_diff>
--- a/src/test/resources/linkedInVisuals/Linkedin Visuals_Omkar.xlsx
+++ b/src/test/resources/linkedInVisuals/Linkedin Visuals_Omkar.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
   <si>
     <t>Raymond James</t>
   </si>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -206,6 +206,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
@@ -652,10 +676,10 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="5"/>
@@ -670,10 +694,10 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="44" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="8"/>
@@ -688,10 +712,10 @@
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="46" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="6"/>
@@ -706,10 +730,10 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="48" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="7"/>

</xml_diff>